<commit_message>
project excel fixture now runs ok
</commit_message>
<xml_diff>
--- a/module-work/src/main/java/org/incodehq/amberg/vshcolab/modules/work/fixture/viewmodel/VSH Sample data.xlsx
+++ b/module-work/src/main/java/org/incodehq/amberg/vshcolab/modules/work/fixture/viewmodel/VSH Sample data.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="645" windowWidth="16935" windowHeight="6855"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Projekt" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>kostenTraeger</t>
   </si>
@@ -99,73 +102,411 @@
   </si>
   <si>
     <t>SN EN 12350-8</t>
+  </si>
+  <si>
+    <t>bericht</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="19" max="19" width="53.71"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
@@ -179,25 +520,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="R2" s="1">
-        <v>13400.0</v>
+        <v>13400</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R3" s="1">
-        <v>13410.0</v>
+        <v>13410</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R4" s="1">
-        <v>13412.0</v>
+        <v>13412</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>15</v>
@@ -206,14 +562,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R6" s="1">
-        <v>13414.0</v>
+        <v>13414</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>19</v>
@@ -222,19 +578,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R9" s="1">
-        <v>13416.0</v>
+        <v>13416</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>24</v>
@@ -243,9 +599,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R10" s="1">
-        <v>13418.0</v>
+        <v>13418</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>25</v>
@@ -254,9 +610,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R11" s="1">
-        <v>13421.0</v>
+        <v>13421</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>27</v>
@@ -266,21 +622,23 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="61.86"/>
+    <col min="4" max="4" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -303,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -327,6 +685,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Norms now have a unit of measurement; tidied up layout of Verfahren
</commit_message>
<xml_diff>
--- a/module-work/src/main/java/org/incodehq/amberg/vshcolab/modules/work/fixture/viewmodel/VSH Sample data.xlsx
+++ b/module-work/src/main/java/org/incodehq/amberg/vshcolab/modules/work/fixture/viewmodel/VSH Sample data.xlsx
@@ -18,12 +18,12 @@
     <sheet name="Sheet5" sheetId="4" r:id="rId4"/>
     <sheet name="Pruefbericht" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="189">
   <si>
     <t>type</t>
   </si>
@@ -575,6 +575,21 @@
   </si>
   <si>
     <t> Stahlschenkel liegen bei der Bestimmung der Prüfkörperabmessungen nicht an (automatische Messstation)</t>
+  </si>
+  <si>
+    <t>normUnitOfMeasurement</t>
+  </si>
+  <si>
+    <t>NOT_APPLICABLE</t>
+  </si>
+  <si>
+    <t>LENGTH_IN_MM</t>
+  </si>
+  <si>
+    <t>DENSITY</t>
+  </si>
+  <si>
+    <t>PERCENTAGE</t>
   </si>
 </sst>
 </file>
@@ -663,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -676,6 +691,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,7 +1009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1057,6 +1076,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1064,14 +1084,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="107" customWidth="1"/>
+    <col min="4" max="4" width="74.28515625" customWidth="1"/>
     <col min="6" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1097,6 +1120,9 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H1" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1">
@@ -1110,6 +1136,7 @@
       <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" s="1">
@@ -1124,6 +1151,7 @@
       <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="1">
@@ -1144,6 +1172,9 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1">
@@ -1151,6 +1182,9 @@
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="H5" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" s="1">
@@ -1171,6 +1205,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1">
@@ -1178,12 +1215,18 @@
       <c r="G7" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="H7" s="13" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="H8" s="13" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="1">
@@ -1205,6 +1248,9 @@
       <c r="G9" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="H9" s="13" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="1">
@@ -1226,6 +1272,9 @@
       <c r="G10" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="H10" s="13" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="1">
@@ -1247,6 +1296,9 @@
       <c r="G11" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H11" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="1">
@@ -1268,6 +1320,9 @@
       <c r="G12" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="H12" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1">
       <c r="A13" s="1">
@@ -1289,6 +1344,9 @@
       <c r="G13" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="H13" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1">
       <c r="A14" s="1">
@@ -1310,6 +1368,9 @@
       <c r="G14" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="H14" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1">
       <c r="A15" s="1">
@@ -1330,6 +1391,9 @@
       </c>
       <c r="G15" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1">
@@ -1513,6 +1577,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1559,7 +1624,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="18">
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
@@ -1619,7 +1684,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" ht="15">
       <c r="A26" s="8" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
renames BusinessVerfahren to Andere, adds in when and who for Durchfuhreung, extends UnitOfMeasurement
</commit_message>
<xml_diff>
--- a/module-work/src/main/java/org/incodehq/amberg/vshcolab/modules/work/fixture/viewmodel/VSH Sample data.xlsx
+++ b/module-work/src/main/java/org/incodehq/amberg/vshcolab/modules/work/fixture/viewmodel/VSH Sample data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="193">
   <si>
     <t>type</t>
   </si>
@@ -580,9 +580,6 @@
     <t>normUnitOfMeasurement</t>
   </si>
   <si>
-    <t>NOT_APPLICABLE</t>
-  </si>
-  <si>
     <t>LENGTH_IN_MM</t>
   </si>
   <si>
@@ -590,13 +587,28 @@
   </si>
   <si>
     <t>PERCENTAGE</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Project definition</t>
+  </si>
+  <si>
+    <t>Project report</t>
+  </si>
+  <si>
+    <t>RATIO</t>
+  </si>
+  <si>
+    <t>TIME_IN_SEC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -642,6 +654,12 @@
       <sz val="11"/>
       <name val="'ArialMT'"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -651,7 +669,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -674,11 +692,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -693,6 +726,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1138,7 +1177,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A3" s="1">
         <v>13410</v>
       </c>
@@ -1153,7 +1192,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="1">
         <v>13412</v>
       </c>
@@ -1173,20 +1212,20 @@
       <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H4" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H5" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="1">
         <v>13414</v>
       </c>
@@ -1206,29 +1245,29 @@
       <c r="G6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H6" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H7" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H8" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A9" s="1">
         <v>13416</v>
       </c>
@@ -1248,11 +1287,11 @@
       <c r="G9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H9" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="1">
         <v>13418</v>
       </c>
@@ -1272,11 +1311,11 @@
       <c r="G10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H10" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A11" s="1">
         <v>13421</v>
       </c>
@@ -1296,11 +1335,11 @@
       <c r="G11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="15" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="1">
         <v>13423</v>
       </c>
@@ -1320,11 +1359,11 @@
       <c r="G12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H12" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A13" s="1">
         <v>13424</v>
       </c>
@@ -1344,11 +1383,11 @@
       <c r="G13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H13" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A14" s="1">
         <v>13426</v>
       </c>
@@ -1368,11 +1407,11 @@
       <c r="G14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1">
+      <c r="H14" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A15" s="1">
         <v>13425</v>
       </c>
@@ -1392,8 +1431,8 @@
       <c r="G15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>185</v>
+      <c r="H15" s="15" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1">
@@ -1497,7 +1536,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
       <c r="A22" s="1">
         <v>13445</v>
       </c>
@@ -1514,18 +1553,34 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A23" s="14">
+        <v>1</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A24" s="14">
+        <v>99999</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>190</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">

</xml_diff>